<commit_message>
Uploading excel file "Classificacao_por_rodada"
</commit_message>
<xml_diff>
--- a/classificacao_por_rodada.xlsx
+++ b/classificacao_por_rodada.xlsx
@@ -17820,23 +17820,23 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Bahia</t>
+          <t>Vasco</t>
         </is>
       </c>
       <c r="D4" t="n">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E4" t="n">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="F4" t="n">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="G4" t="n">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="H4" t="n">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5">
@@ -17848,23 +17848,23 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Vasco</t>
+          <t>Bahia</t>
         </is>
       </c>
       <c r="D5" t="n">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E5" t="n">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="F5" t="n">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="G5" t="n">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="H5" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6">
@@ -17880,7 +17880,7 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E6" t="n">
         <v>31</v>
@@ -17920,7 +17920,7 @@
         <v>5</v>
       </c>
       <c r="H7" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8">
@@ -17948,7 +17948,7 @@
         <v>11</v>
       </c>
       <c r="H8" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9">
@@ -18004,7 +18004,7 @@
         <v>1</v>
       </c>
       <c r="H10" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11">
@@ -18088,7 +18088,7 @@
         <v>-2</v>
       </c>
       <c r="H13" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="14">
@@ -18116,7 +18116,7 @@
         <v>-5</v>
       </c>
       <c r="H14" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="15">
@@ -18172,7 +18172,7 @@
         <v>-5</v>
       </c>
       <c r="H16" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="17">
@@ -18440,7 +18440,7 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="E4" t="n">
         <v>45</v>
@@ -18536,7 +18536,7 @@
         <v>2</v>
       </c>
       <c r="H7" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8">
@@ -18552,7 +18552,7 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E8" t="n">
         <v>32</v>
@@ -18592,7 +18592,7 @@
         <v>4</v>
       </c>
       <c r="H9" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10">
@@ -18620,7 +18620,7 @@
         <v>10</v>
       </c>
       <c r="H10" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11">
@@ -18676,7 +18676,7 @@
         <v>-4</v>
       </c>
       <c r="H12" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13">
@@ -18704,7 +18704,7 @@
         <v>-2</v>
       </c>
       <c r="H13" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="14">
@@ -18816,7 +18816,7 @@
         <v>-5</v>
       </c>
       <c r="H17" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="18">
@@ -19052,20 +19052,20 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Bahia</t>
+          <t>Vasco</t>
         </is>
       </c>
       <c r="D4" t="n">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="E4" t="n">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="F4" t="n">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="G4" t="n">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="H4" t="n">
         <v>16</v>
@@ -19080,20 +19080,20 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Vasco</t>
+          <t>Bahia</t>
         </is>
       </c>
       <c r="D5" t="n">
         <v>59</v>
       </c>
       <c r="E5" t="n">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="F5" t="n">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="G5" t="n">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="H5" t="n">
         <v>16</v>
@@ -19140,7 +19140,7 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E7" t="n">
         <v>37</v>
@@ -19180,7 +19180,7 @@
         <v>5</v>
       </c>
       <c r="H8" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9">
@@ -19208,7 +19208,7 @@
         <v>0</v>
       </c>
       <c r="H9" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10">
@@ -19236,7 +19236,7 @@
         <v>10</v>
       </c>
       <c r="H10" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11">
@@ -19292,7 +19292,7 @@
         <v>-4</v>
       </c>
       <c r="H12" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13">
@@ -19348,7 +19348,7 @@
         <v>-3</v>
       </c>
       <c r="H14" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="15">
@@ -19460,7 +19460,7 @@
         <v>-8</v>
       </c>
       <c r="H18" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="19">
@@ -19668,20 +19668,20 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Bahia</t>
+          <t>Vasco</t>
         </is>
       </c>
       <c r="D4" t="n">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="E4" t="n">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="F4" t="n">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="G4" t="n">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="H4" t="n">
         <v>17</v>
@@ -19696,20 +19696,20 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Vasco</t>
+          <t>Bahia</t>
         </is>
       </c>
       <c r="D5" t="n">
         <v>62</v>
       </c>
       <c r="E5" t="n">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="F5" t="n">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="G5" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="H5" t="n">
         <v>17</v>
@@ -19740,7 +19740,7 @@
         <v>6</v>
       </c>
       <c r="H6" t="n">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7">
@@ -19784,7 +19784,7 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E8" t="n">
         <v>37</v>
@@ -19824,7 +19824,7 @@
         <v>12</v>
       </c>
       <c r="H9" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10">
@@ -19852,7 +19852,7 @@
         <v>-1</v>
       </c>
       <c r="H10" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="11">
@@ -19880,7 +19880,7 @@
         <v>-3</v>
       </c>
       <c r="H11" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="12">
@@ -19964,7 +19964,7 @@
         <v>-3</v>
       </c>
       <c r="H14" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="15">
@@ -20048,7 +20048,7 @@
         <v>-5</v>
       </c>
       <c r="H17" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="18">

</xml_diff>